<commit_message>
[#959] Put IDName in default_configuration to allow spreadsheet override
Requires an as yet unmerged flatten-tool commit
https://github.com/OpenDataServices/flatten-tool/pull/219
</commit_message>
<xml_diff>
--- a/cove_iati/fixtures/basic_iati_org_valid.xlsx
+++ b/cove_iati/fixtures/basic_iati_org_valid.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Meta" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Meta" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,11 +23,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+  <si>
+    <t xml:space="preserve">#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XMLRootTag iati-organisations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RootListPath iati-organisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDName organisation-identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@version</t>
+  </si>
   <si>
     <t xml:space="preserve">organisation-identifier</t>
   </si>
   <si>
+    <t xml:space="preserve">@xml:lang</t>
+  </si>
+  <si>
     <t xml:space="preserve">@last-updated-datetime</t>
   </si>
   <si>
@@ -47,6 +67,9 @@
     <t xml:space="preserve">AA-AAA-123456789</t>
   </si>
   <si>
+    <t xml:space="preserve">en</t>
+  </si>
+  <si>
     <t xml:space="preserve">2014-09-10T07:15:37Z</t>
   </si>
   <si>
@@ -56,26 +79,81 @@
     <t xml:space="preserve">Organisation name</t>
   </si>
   <si>
-    <t xml:space="preserve">#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XMLRootTag iati-organisations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RootListPath iati-organisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@version</t>
+    <t xml:space="preserve">document-link/0/@url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document-link/0/@format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document-link/0/title/narrative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document-link/0/title/narrative/@xml:lang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document-link/0/category/0/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document-link/0/language/0/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document-link/0/document-date/@iso-date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document-link/recipient-country/@code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.example.org/docs/report_en.odt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">application/vnd.oasis.opendocument.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual Report 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AF</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">http://www.example.org/docs/report_fr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.odt</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Rapport annuel 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -96,6 +174,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,12 +225,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -166,74 +267,133 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -247,45 +407,139 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>2.03</v>
+      <c r="H2" s="4" t="n">
+        <v>41675</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="46.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>41675</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="http://www.example.org/docs/report_fr"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Fix headings in basic_iati_org_valid.xlsx spreadsheet
</commit_message>
<xml_diff>
--- a/cove_iati/fixtures/basic_iati_org_valid.xlsx
+++ b/cove_iati/fixtures/basic_iati_org_valid.xlsx
@@ -5,13 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -85,10 +84,10 @@
     <t xml:space="preserve">document-link/0/@format</t>
   </si>
   <si>
-    <t xml:space="preserve">document-link/0/title/narrative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">document-link/0/title/narrative/@xml:lang</t>
+    <t xml:space="preserve">document-link/0/title/0/narrative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document-link/0/title/0/narrative/@xml:lang</t>
   </si>
   <si>
     <t xml:space="preserve">document-link/0/category/0/@code</t>
@@ -100,7 +99,7 @@
     <t xml:space="preserve">document-link/0/document-date/@iso-date</t>
   </si>
   <si>
-    <t xml:space="preserve">document-link/recipient-country/@code</t>
+    <t xml:space="preserve">document-link/0/recipient-country/@code</t>
   </si>
   <si>
     <t xml:space="preserve">http://www.example.org/docs/report_en.odt</t>
@@ -118,25 +117,7 @@
     <t xml:space="preserve">AF</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://www.example.org/docs/report_fr</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.odt</t>
-    </r>
+    <t xml:space="preserve">http://www.example.org/docs/report_fr.odt</t>
   </si>
   <si>
     <t xml:space="preserve">Rapport annuel 2013</t>
@@ -225,7 +206,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,6 +221,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -269,16 +254,16 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1887755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -328,20 +313,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.1989795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -414,15 +397,14 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4642857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,7 +432,7 @@
       <c r="H1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -474,7 +456,7 @@
       <c r="G2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="n">
+      <c r="H2" s="5" t="n">
         <v>41675</v>
       </c>
       <c r="I2" s="0" t="s">
@@ -485,7 +467,7 @@
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -503,7 +485,7 @@
       <c r="G3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="4" t="n">
+      <c r="H3" s="5" t="n">
         <v>41675</v>
       </c>
       <c r="I3" s="0" t="s">
@@ -512,7 +494,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="http://www.example.org/docs/report_fr"/>
+    <hyperlink ref="B3" r:id="rId1" display="http://www.example.org/docs/report_fr.odt"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -522,30 +504,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>